<commit_message>
Added a testjobs for new function read_ts_xlsx and read_ts_csv.
</commit_message>
<xml_diff>
--- a/examples/read_ts/xlsx/example2.xlsx
+++ b/examples/read_ts/xlsx/example2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="first_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">The data is on the next sheet </t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">Timeseries a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeseries b in euros</t>
   </si>
   <si>
     <t xml:space="preserve">b</t>
@@ -63,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +90,13 @@
     </font>
     <font>
       <sz val="96"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -134,12 +144,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,13 +176,13 @@
   </sheetPr>
   <dimension ref="B9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.2142857142857"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="114.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,21 +206,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.56632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="12.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.63775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,22 +261,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
read_ts_xlsx now reads exactly as many columns as the determined column types.
</commit_message>
<xml_diff>
--- a/examples/read_ts/xlsx/example2.xlsx
+++ b/examples/read_ts/xlsx/example2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="first_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">The data is on the next sheet </t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Timeseries b in euros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jan</t>
   </si>
   <si>
     <t xml:space="preserve">b</t>
@@ -182,7 +185,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="114.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,22 +209,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.63775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,16 +267,19 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J5" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>10</v>

</xml_diff>